<commit_message>
last edit and creat a same report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/loginData.xlsx
+++ b/src/test/resources/testdata/loginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A4430C90-E937-4119-8E89-7F5A3B1374B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9F7FFBB9-31BD-4FC0-B094-C0DEE58B5167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Email</t>
   </si>
@@ -54,19 +54,12 @@
   </si>
   <si>
     <t>SKIPPED</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,10 +114,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -409,14 +402,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="52.77734375"/>
-    <col min="2" max="2" customWidth="true" width="91.0"/>
+    <col min="1" max="1" width="52.77734375" customWidth="1"/>
+    <col min="2" max="2" width="91" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -444,7 +437,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -456,7 +449,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -470,7 +463,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -482,7 +475,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
addcart and login (not finish)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/loginData.xlsx
+++ b/src/test/resources/testdata/loginData.xlsx
@@ -3,15 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9F7FFBB9-31BD-4FC0-B094-C0DEE58B5167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\eclipse-workspace\frontgate-tests\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE33D6EF-5039-4393-B731-77FC6D20D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Products" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Email</t>
   </si>
@@ -29,38 +34,68 @@
     <t>Password</t>
   </si>
   <si>
-    <t>WrongPass$123</t>
+    <t>RunFlag</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>ahmadj7hanani0@gmail.com</t>
   </si>
   <si>
     <t>0569630981Aa$</t>
   </si>
   <si>
-    <t>RunFlag</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>ahmadj7hanani0@gmail</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
-    <t>ahmad@@gmail</t>
-  </si>
-  <si>
-    <t>ERROR</t>
-  </si>
-  <si>
-    <t>SKIPPED</t>
+    <t>ahmad@gmail.com</t>
+  </si>
+  <si>
+    <t>0569630981Aa$4</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Frontgate Resort Collection™ Bath Towels</t>
+  </si>
+  <si>
+    <t>Bath Towel</t>
+  </si>
+  <si>
+    <t>Chiffon</t>
+  </si>
+  <si>
+    <t>Bath Mat</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>Resort Bath Sheet</t>
+  </si>
+  <si>
+    <t>Bath Sheet</t>
+  </si>
+  <si>
+    <t>White</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +107,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,19 +152,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,17 +450,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.77734375" customWidth="1"/>
-    <col min="2" max="2" width="91" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,75 +469,162 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="mailto:ahmadj7hanani0@gmail.com" xr:uid="{3995E7E8-73FD-48C9-8F0C-D84E9D966214}"/>
+    <hyperlink ref="A3" r:id="rId2" display="mailto:ahmad@gmail.com" xr:uid="{EA1A1564-25AC-43F0-84C4-3AB61E0296C8}"/>
+    <hyperlink ref="A4" r:id="rId3" display="mailto:ahmadj7hanani0@gmail.com" xr:uid="{60B0BD1E-7F0C-4BF1-BEDD-EB1C2403E9EA}"/>
+    <hyperlink ref="A6" r:id="rId4" display="mailto:ahmadj7hanani0@gmail.com" xr:uid="{4B39E79F-3304-47B2-8E43-89F7CA154CB7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4B50ED-D640-4882-962A-B87D9E6522A9}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>